<commit_message>
Adicao de algumas funcoes adicionais reponsaveis pela conversao do formato das rotas.
</commit_message>
<xml_diff>
--- a/Saida.xlsx
+++ b/Saida.xlsx
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,10 +395,10 @@
         <v>0.5</v>
       </c>
       <c r="E1">
-        <v>3728.080175597796</v>
+        <v>3918.965007467933</v>
       </c>
       <c r="F1">
-        <v>0.8917135444361982</v>
+        <v>0.8744726293774652</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -409,10 +409,10 @@
         <v>50</v>
       </c>
       <c r="E2">
-        <v>3638.601827784942</v>
+        <v>4046.226505918316</v>
       </c>
       <c r="F2">
-        <v>0.8871011604741776</v>
+        <v>0.8771926484679836</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -423,10 +423,10 @@
         <v>25</v>
       </c>
       <c r="E3">
-        <v>3692.440904402963</v>
+        <v>4000.938865799878</v>
       </c>
       <c r="F3">
-        <v>0.8881636852200203</v>
+        <v>0.8761829498419887</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -437,10 +437,10 @@
         <v>50</v>
       </c>
       <c r="E4">
-        <v>3680.244440748373</v>
+        <v>3657.135991387497</v>
       </c>
       <c r="F4">
-        <v>0.8880123725841921</v>
+        <v>0.8638507711238541</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -451,18 +451,18 @@
         <v>30</v>
       </c>
       <c r="E5">
-        <v>3628.332399934083</v>
+        <v>3691.662049029868</v>
       </c>
       <c r="F5">
-        <v>0.8826256914650515</v>
+        <v>0.8667998525276273</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="E6">
-        <v>3632.221592752433</v>
+        <v>3743.48109539564</v>
       </c>
       <c r="F6">
-        <v>0.8849690375097699</v>
+        <v>0.8710824545673868</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -473,10 +473,10 @@
         <v>100</v>
       </c>
       <c r="E7">
-        <v>3678.893127453969</v>
+        <v>4075.612340139283</v>
       </c>
       <c r="F7">
-        <v>0.8879404635511657</v>
+        <v>0.8773679444291423</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -487,10 +487,18 @@
         <v>5</v>
       </c>
       <c r="E8">
-        <v>3696.095224496501</v>
+        <v>3649.317874322935</v>
       </c>
       <c r="F8">
-        <v>0.8890152846186632</v>
+        <v>0.8609585078099218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="E9">
+        <v>3936.104497130708</v>
+      </c>
+      <c r="F9">
+        <v>0.8750245789681041</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -500,6 +508,12 @@
       <c r="B10">
         <v>0.75</v>
       </c>
+      <c r="E10">
+        <v>3957.666379190404</v>
+      </c>
+      <c r="F10">
+        <v>0.875905878642028</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -508,6 +522,12 @@
       <c r="B11">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>3773.551720558038</v>
+      </c>
+      <c r="F11">
+        <v>0.8718342842150564</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -516,6 +536,12 @@
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="E12">
+        <v>4002.437914321994</v>
+      </c>
+      <c r="F12">
+        <v>0.8765861657046756</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
@@ -523,6 +549,28 @@
       </c>
       <c r="B13">
         <v>2</v>
+      </c>
+      <c r="E13">
+        <v>3884.662082949515</v>
+      </c>
+      <c r="F13">
+        <v>0.8743602821837185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="E14">
+        <v>3939.123864467525</v>
+      </c>
+      <c r="F14">
+        <v>0.8758262600701566</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="E15">
+        <v>3794.989528581777</v>
+      </c>
+      <c r="F15">
+        <v>0.8737554517519703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>